<commit_message>
Moved xCommand files from Common directory, major bugfixes of ecu processing, sensors error handling, new configuration tables
</commit_message>
<xml_diff>
--- a/Docs/Injection table - precalculated.xlsx
+++ b/Docs/Injection table - precalculated.xlsx
@@ -351,8 +351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:P55"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1509,10 +1509,10 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="B28">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1559,13 +1559,13 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="B29">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1609,13 +1609,13 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1659,19 +1659,19 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="B31">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1709,19 +1709,19 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="B32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1759,19 +1759,19 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="B33">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1809,19 +1809,19 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="B34">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1859,19 +1859,19 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="B35">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -1909,19 +1909,19 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="B36">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2356,7 +2356,7 @@
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
-        <v>152.68</v>
+        <v>169.64</v>
       </c>
       <c r="B46">
         <f t="shared" si="1"/>
@@ -2422,11 +2422,11 @@
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
-        <v>155.1</v>
+        <v>193.88</v>
       </c>
       <c r="B47">
         <f t="shared" si="1"/>
-        <v>174.49</v>
+        <v>193.88</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
@@ -2488,15 +2488,15 @@
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
-        <v>152.68</v>
+        <v>218.11</v>
       </c>
       <c r="B48">
         <f t="shared" si="1"/>
-        <v>174.49</v>
+        <v>218.11</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>196.3</v>
+        <v>218.11</v>
       </c>
       <c r="D48">
         <f t="shared" si="1"/>
@@ -2554,15 +2554,15 @@
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
-        <v>145.4</v>
+        <v>242.34</v>
       </c>
       <c r="B49">
         <f t="shared" si="1"/>
-        <v>169.64</v>
+        <v>242.34</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>193.87</v>
+        <v>242.34</v>
       </c>
       <c r="D49">
         <f t="shared" si="1"/>
@@ -2620,23 +2620,23 @@
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
-        <v>133.29</v>
+        <v>266.58</v>
       </c>
       <c r="B50">
         <f t="shared" si="1"/>
-        <v>159.94999999999999</v>
+        <v>266.58</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>186.61</v>
+        <v>266.58</v>
       </c>
       <c r="D50">
         <f t="shared" si="1"/>
-        <v>239.92</v>
+        <v>266.58</v>
       </c>
       <c r="E50">
         <f t="shared" si="1"/>
-        <v>239.92</v>
+        <v>266.58</v>
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
@@ -2686,23 +2686,23 @@
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
-        <v>116.32</v>
+        <v>290.81</v>
       </c>
       <c r="B51">
         <f t="shared" si="1"/>
-        <v>145.41</v>
+        <v>290.81</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>174.49</v>
+        <v>290.81</v>
       </c>
       <c r="D51">
         <f t="shared" si="1"/>
-        <v>232.65</v>
+        <v>290.81</v>
       </c>
       <c r="E51">
         <f t="shared" si="1"/>
-        <v>261.73</v>
+        <v>290.81</v>
       </c>
       <c r="F51">
         <f t="shared" si="1"/>
@@ -2752,23 +2752,23 @@
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
-        <v>126.02</v>
+        <v>315.05</v>
       </c>
       <c r="B52">
         <f t="shared" si="1"/>
-        <v>141.77000000000001</v>
+        <v>315.05</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>157.53</v>
+        <v>315.05</v>
       </c>
       <c r="D52">
         <f t="shared" si="1"/>
-        <v>220.54</v>
+        <v>315.05</v>
       </c>
       <c r="E52">
         <f t="shared" si="1"/>
-        <v>252.04</v>
+        <v>315.05</v>
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
@@ -2818,23 +2818,23 @@
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
-        <v>135.71</v>
+        <v>339.28</v>
       </c>
       <c r="B53">
         <f t="shared" si="1"/>
-        <v>135.71</v>
+        <v>339.28</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>135.71</v>
+        <v>339.28</v>
       </c>
       <c r="D53">
         <f t="shared" si="1"/>
-        <v>203.57</v>
+        <v>339.28</v>
       </c>
       <c r="E53">
         <f t="shared" si="1"/>
-        <v>271.42</v>
+        <v>339.28</v>
       </c>
       <c r="F53">
         <f t="shared" si="1"/>
@@ -2884,23 +2884,23 @@
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
-        <v>145.41</v>
+        <v>363.52</v>
       </c>
       <c r="B54">
         <f t="shared" si="1"/>
-        <v>145.41</v>
+        <v>363.52</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>145.41</v>
+        <v>363.52</v>
       </c>
       <c r="D54">
         <f t="shared" si="1"/>
-        <v>218.11</v>
+        <v>363.52</v>
       </c>
       <c r="E54">
         <f t="shared" si="1"/>
-        <v>290.82</v>
+        <v>363.52</v>
       </c>
       <c r="F54">
         <f t="shared" si="1"/>
@@ -2950,23 +2950,23 @@
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
-        <v>155.1</v>
+        <v>387.75</v>
       </c>
       <c r="B55">
         <f t="shared" si="1"/>
-        <v>155.1</v>
+        <v>387.75</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>155.1</v>
+        <v>387.75</v>
       </c>
       <c r="D55">
         <f t="shared" si="1"/>
-        <v>232.65</v>
+        <v>387.75</v>
       </c>
       <c r="E55">
         <f t="shared" si="1"/>
-        <v>310.2</v>
+        <v>387.75</v>
       </c>
       <c r="F55">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
THR to MAP is now in kPa instead of bar
</commit_message>
<xml_diff>
--- a/Docs/Injection table - precalculated.xlsx
+++ b/Docs/Injection table - precalculated.xlsx
@@ -12,6 +12,14 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>0.1</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="N4" workbookViewId="0">
+      <selection activeCell="Y21" sqref="Y21:AN36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1165,7 @@
         <v>387.75</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1206,8 +1214,65 @@
       <c r="P21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21" t="s">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>6.3328124999999999E-2</v>
+      </c>
+      <c r="Y21">
+        <v>0.5</v>
+      </c>
+      <c r="Z21">
+        <v>0.4</v>
+      </c>
+      <c r="AA21">
+        <v>0.2</v>
+      </c>
+      <c r="AB21">
+        <v>0.06</v>
+      </c>
+      <c r="AC21">
+        <v>0.06</v>
+      </c>
+      <c r="AD21">
+        <v>0.06</v>
+      </c>
+      <c r="AE21">
+        <v>0.06</v>
+      </c>
+      <c r="AF21">
+        <v>0.06</v>
+      </c>
+      <c r="AG21">
+        <v>0.06</v>
+      </c>
+      <c r="AH21">
+        <v>0.06</v>
+      </c>
+      <c r="AI21">
+        <v>0.06</v>
+      </c>
+      <c r="AJ21">
+        <v>0.06</v>
+      </c>
+      <c r="AK21">
+        <v>0.06</v>
+      </c>
+      <c r="AL21">
+        <v>0.06</v>
+      </c>
+      <c r="AM21">
+        <v>0.06</v>
+      </c>
+      <c r="AN21">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1256,8 +1321,62 @@
       <c r="P22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S22">
+        <v>2</v>
+      </c>
+      <c r="W22">
+        <v>0.12665625</v>
+      </c>
+      <c r="Y22">
+        <v>0.5</v>
+      </c>
+      <c r="Z22">
+        <v>0.4</v>
+      </c>
+      <c r="AA22">
+        <v>0.25</v>
+      </c>
+      <c r="AB22">
+        <v>0.13</v>
+      </c>
+      <c r="AC22">
+        <v>0.13</v>
+      </c>
+      <c r="AD22">
+        <v>0.13</v>
+      </c>
+      <c r="AE22">
+        <v>0.13</v>
+      </c>
+      <c r="AF22">
+        <v>0.13</v>
+      </c>
+      <c r="AG22">
+        <v>0.13</v>
+      </c>
+      <c r="AH22">
+        <v>0.13</v>
+      </c>
+      <c r="AI22">
+        <v>0.13</v>
+      </c>
+      <c r="AJ22">
+        <v>0.13</v>
+      </c>
+      <c r="AK22">
+        <v>0.13</v>
+      </c>
+      <c r="AL22">
+        <v>0.13</v>
+      </c>
+      <c r="AM22">
+        <v>0.13</v>
+      </c>
+      <c r="AN22">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1306,8 +1425,62 @@
       <c r="P23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S23">
+        <v>3</v>
+      </c>
+      <c r="W23">
+        <v>0.18998437499999998</v>
+      </c>
+      <c r="Y23">
+        <v>0.5</v>
+      </c>
+      <c r="Z23">
+        <v>0.4</v>
+      </c>
+      <c r="AA23">
+        <v>0.3</v>
+      </c>
+      <c r="AB23">
+        <v>0.19</v>
+      </c>
+      <c r="AC23">
+        <v>0.19</v>
+      </c>
+      <c r="AD23">
+        <v>0.19</v>
+      </c>
+      <c r="AE23">
+        <v>0.19</v>
+      </c>
+      <c r="AF23">
+        <v>0.19</v>
+      </c>
+      <c r="AG23">
+        <v>0.19</v>
+      </c>
+      <c r="AH23">
+        <v>0.19</v>
+      </c>
+      <c r="AI23">
+        <v>0.19</v>
+      </c>
+      <c r="AJ23">
+        <v>0.19</v>
+      </c>
+      <c r="AK23">
+        <v>0.19</v>
+      </c>
+      <c r="AL23">
+        <v>0.19</v>
+      </c>
+      <c r="AM23">
+        <v>0.19</v>
+      </c>
+      <c r="AN23">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1356,8 +1529,62 @@
       <c r="P24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S24">
+        <v>4</v>
+      </c>
+      <c r="W24">
+        <v>0.2533125</v>
+      </c>
+      <c r="Y24">
+        <v>0.5</v>
+      </c>
+      <c r="Z24">
+        <v>0.4</v>
+      </c>
+      <c r="AA24">
+        <v>0.35</v>
+      </c>
+      <c r="AB24">
+        <v>0.25</v>
+      </c>
+      <c r="AC24">
+        <v>0.25</v>
+      </c>
+      <c r="AD24">
+        <v>0.25</v>
+      </c>
+      <c r="AE24">
+        <v>0.25</v>
+      </c>
+      <c r="AF24">
+        <v>0.25</v>
+      </c>
+      <c r="AG24">
+        <v>0.25</v>
+      </c>
+      <c r="AH24">
+        <v>0.25</v>
+      </c>
+      <c r="AI24">
+        <v>0.25</v>
+      </c>
+      <c r="AJ24">
+        <v>0.25</v>
+      </c>
+      <c r="AK24">
+        <v>0.25</v>
+      </c>
+      <c r="AL24">
+        <v>0.25</v>
+      </c>
+      <c r="AM24">
+        <v>0.25</v>
+      </c>
+      <c r="AN24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1406,8 +1633,62 @@
       <c r="P25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S25">
+        <v>5</v>
+      </c>
+      <c r="W25">
+        <v>0.31664062500000001</v>
+      </c>
+      <c r="Y25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Z25">
+        <v>0.5</v>
+      </c>
+      <c r="AA25">
+        <v>0.4</v>
+      </c>
+      <c r="AB25">
+        <v>0.32</v>
+      </c>
+      <c r="AC25">
+        <v>0.32</v>
+      </c>
+      <c r="AD25">
+        <v>0.32</v>
+      </c>
+      <c r="AE25">
+        <v>0.32</v>
+      </c>
+      <c r="AF25">
+        <v>0.32</v>
+      </c>
+      <c r="AG25">
+        <v>0.32</v>
+      </c>
+      <c r="AH25">
+        <v>0.32</v>
+      </c>
+      <c r="AI25">
+        <v>0.32</v>
+      </c>
+      <c r="AJ25">
+        <v>0.32</v>
+      </c>
+      <c r="AK25">
+        <v>0.32</v>
+      </c>
+      <c r="AL25">
+        <v>0.32</v>
+      </c>
+      <c r="AM25">
+        <v>0.32</v>
+      </c>
+      <c r="AN25">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1456,8 +1737,62 @@
       <c r="P26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S26">
+        <v>6</v>
+      </c>
+      <c r="W26">
+        <v>0.37996874999999997</v>
+      </c>
+      <c r="Y26">
+        <v>0.6</v>
+      </c>
+      <c r="Z26">
+        <v>0.5</v>
+      </c>
+      <c r="AA26">
+        <v>0.45</v>
+      </c>
+      <c r="AB26">
+        <v>0.38</v>
+      </c>
+      <c r="AC26">
+        <v>0.38</v>
+      </c>
+      <c r="AD26">
+        <v>0.38</v>
+      </c>
+      <c r="AE26">
+        <v>0.38</v>
+      </c>
+      <c r="AF26">
+        <v>0.38</v>
+      </c>
+      <c r="AG26">
+        <v>0.38</v>
+      </c>
+      <c r="AH26">
+        <v>0.38</v>
+      </c>
+      <c r="AI26">
+        <v>0.38</v>
+      </c>
+      <c r="AJ26">
+        <v>0.38</v>
+      </c>
+      <c r="AK26">
+        <v>0.38</v>
+      </c>
+      <c r="AL26">
+        <v>0.38</v>
+      </c>
+      <c r="AM26">
+        <v>0.38</v>
+      </c>
+      <c r="AN26">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1506,8 +1841,62 @@
       <c r="P27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S27">
+        <v>7</v>
+      </c>
+      <c r="W27">
+        <v>0.44329687499999998</v>
+      </c>
+      <c r="Y27">
+        <v>0.65</v>
+      </c>
+      <c r="Z27">
+        <v>0.6</v>
+      </c>
+      <c r="AA27">
+        <v>0.5</v>
+      </c>
+      <c r="AB27">
+        <v>0.44</v>
+      </c>
+      <c r="AC27">
+        <v>0.44</v>
+      </c>
+      <c r="AD27">
+        <v>0.44</v>
+      </c>
+      <c r="AE27">
+        <v>0.44</v>
+      </c>
+      <c r="AF27">
+        <v>0.44</v>
+      </c>
+      <c r="AG27">
+        <v>0.44</v>
+      </c>
+      <c r="AH27">
+        <v>0.44</v>
+      </c>
+      <c r="AI27">
+        <v>0.44</v>
+      </c>
+      <c r="AJ27">
+        <v>0.44</v>
+      </c>
+      <c r="AK27">
+        <v>0.44</v>
+      </c>
+      <c r="AL27">
+        <v>0.44</v>
+      </c>
+      <c r="AM27">
+        <v>0.44</v>
+      </c>
+      <c r="AN27">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1556,8 +1945,62 @@
       <c r="P28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S28">
+        <v>8</v>
+      </c>
+      <c r="W28">
+        <v>0.50662499999999999</v>
+      </c>
+      <c r="Y28">
+        <v>0.7</v>
+      </c>
+      <c r="Z28">
+        <v>0.65</v>
+      </c>
+      <c r="AA28">
+        <v>0.65</v>
+      </c>
+      <c r="AB28">
+        <v>0.51</v>
+      </c>
+      <c r="AC28">
+        <v>0.51</v>
+      </c>
+      <c r="AD28">
+        <v>0.51</v>
+      </c>
+      <c r="AE28">
+        <v>0.51</v>
+      </c>
+      <c r="AF28">
+        <v>0.51</v>
+      </c>
+      <c r="AG28">
+        <v>0.51</v>
+      </c>
+      <c r="AH28">
+        <v>0.51</v>
+      </c>
+      <c r="AI28">
+        <v>0.51</v>
+      </c>
+      <c r="AJ28">
+        <v>0.51</v>
+      </c>
+      <c r="AK28">
+        <v>0.51</v>
+      </c>
+      <c r="AL28">
+        <v>0.51</v>
+      </c>
+      <c r="AM28">
+        <v>0.51</v>
+      </c>
+      <c r="AN28">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1606,8 +2049,62 @@
       <c r="P29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S29">
+        <v>9</v>
+      </c>
+      <c r="W29">
+        <v>0.56995312499999995</v>
+      </c>
+      <c r="Y29">
+        <v>0.8</v>
+      </c>
+      <c r="Z29">
+        <v>0.7</v>
+      </c>
+      <c r="AA29">
+        <v>0.6</v>
+      </c>
+      <c r="AB29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AC29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AD29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AE29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AF29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AG29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AH29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AI29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AJ29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AK29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AL29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AM29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AN29">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1656,8 +2153,62 @@
       <c r="P30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S30">
+        <v>10</v>
+      </c>
+      <c r="W30">
+        <v>0.63328125000000002</v>
+      </c>
+      <c r="Y30">
+        <v>0.9</v>
+      </c>
+      <c r="Z30">
+        <v>0.8</v>
+      </c>
+      <c r="AA30">
+        <v>0.7</v>
+      </c>
+      <c r="AB30">
+        <v>0.63</v>
+      </c>
+      <c r="AC30">
+        <v>0.63</v>
+      </c>
+      <c r="AD30">
+        <v>0.63</v>
+      </c>
+      <c r="AE30">
+        <v>0.63</v>
+      </c>
+      <c r="AF30">
+        <v>0.63</v>
+      </c>
+      <c r="AG30">
+        <v>0.63</v>
+      </c>
+      <c r="AH30">
+        <v>0.63</v>
+      </c>
+      <c r="AI30">
+        <v>0.63</v>
+      </c>
+      <c r="AJ30">
+        <v>0.63</v>
+      </c>
+      <c r="AK30">
+        <v>0.63</v>
+      </c>
+      <c r="AL30">
+        <v>0.63</v>
+      </c>
+      <c r="AM30">
+        <v>0.63</v>
+      </c>
+      <c r="AN30">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1706,8 +2257,62 @@
       <c r="P31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S31">
+        <v>11</v>
+      </c>
+      <c r="W31">
+        <v>0.69660937499999998</v>
+      </c>
+      <c r="Y31">
+        <v>1</v>
+      </c>
+      <c r="Z31">
+        <v>0.9</v>
+      </c>
+      <c r="AA31">
+        <v>0.75</v>
+      </c>
+      <c r="AB31">
+        <v>0.7</v>
+      </c>
+      <c r="AC31">
+        <v>0.7</v>
+      </c>
+      <c r="AD31">
+        <v>0.7</v>
+      </c>
+      <c r="AE31">
+        <v>0.7</v>
+      </c>
+      <c r="AF31">
+        <v>0.7</v>
+      </c>
+      <c r="AG31">
+        <v>0.7</v>
+      </c>
+      <c r="AH31">
+        <v>0.7</v>
+      </c>
+      <c r="AI31">
+        <v>0.7</v>
+      </c>
+      <c r="AJ31">
+        <v>0.7</v>
+      </c>
+      <c r="AK31">
+        <v>0.7</v>
+      </c>
+      <c r="AL31">
+        <v>0.7</v>
+      </c>
+      <c r="AM31">
+        <v>0.7</v>
+      </c>
+      <c r="AN31">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1756,8 +2361,62 @@
       <c r="P32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S32">
+        <v>12</v>
+      </c>
+      <c r="W32">
+        <v>0.75993749999999993</v>
+      </c>
+      <c r="Y32">
+        <v>1</v>
+      </c>
+      <c r="Z32">
+        <v>0.9</v>
+      </c>
+      <c r="AA32">
+        <v>0.8</v>
+      </c>
+      <c r="AB32">
+        <v>0.76</v>
+      </c>
+      <c r="AC32">
+        <v>0.76</v>
+      </c>
+      <c r="AD32">
+        <v>0.76</v>
+      </c>
+      <c r="AE32">
+        <v>0.76</v>
+      </c>
+      <c r="AF32">
+        <v>0.76</v>
+      </c>
+      <c r="AG32">
+        <v>0.76</v>
+      </c>
+      <c r="AH32">
+        <v>0.76</v>
+      </c>
+      <c r="AI32">
+        <v>0.76</v>
+      </c>
+      <c r="AJ32">
+        <v>0.76</v>
+      </c>
+      <c r="AK32">
+        <v>0.76</v>
+      </c>
+      <c r="AL32">
+        <v>0.76</v>
+      </c>
+      <c r="AM32">
+        <v>0.76</v>
+      </c>
+      <c r="AN32">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1806,8 +2465,62 @@
       <c r="P33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S33">
+        <v>13</v>
+      </c>
+      <c r="W33">
+        <v>0.823265625</v>
+      </c>
+      <c r="Y33">
+        <v>1</v>
+      </c>
+      <c r="Z33">
+        <v>0.95</v>
+      </c>
+      <c r="AA33">
+        <v>0.9</v>
+      </c>
+      <c r="AB33">
+        <v>0.82</v>
+      </c>
+      <c r="AC33">
+        <v>0.82</v>
+      </c>
+      <c r="AD33">
+        <v>0.82</v>
+      </c>
+      <c r="AE33">
+        <v>0.82</v>
+      </c>
+      <c r="AF33">
+        <v>0.82</v>
+      </c>
+      <c r="AG33">
+        <v>0.82</v>
+      </c>
+      <c r="AH33">
+        <v>0.82</v>
+      </c>
+      <c r="AI33">
+        <v>0.82</v>
+      </c>
+      <c r="AJ33">
+        <v>0.82</v>
+      </c>
+      <c r="AK33">
+        <v>0.82</v>
+      </c>
+      <c r="AL33">
+        <v>0.82</v>
+      </c>
+      <c r="AM33">
+        <v>0.82</v>
+      </c>
+      <c r="AN33">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1856,8 +2569,62 @@
       <c r="P34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S34">
+        <v>14</v>
+      </c>
+      <c r="W34">
+        <v>0.88659374999999996</v>
+      </c>
+      <c r="Y34">
+        <v>1</v>
+      </c>
+      <c r="Z34">
+        <v>0.97</v>
+      </c>
+      <c r="AA34">
+        <v>0.95</v>
+      </c>
+      <c r="AB34">
+        <v>0.89</v>
+      </c>
+      <c r="AC34">
+        <v>0.89</v>
+      </c>
+      <c r="AD34">
+        <v>0.89</v>
+      </c>
+      <c r="AE34">
+        <v>0.89</v>
+      </c>
+      <c r="AF34">
+        <v>0.89</v>
+      </c>
+      <c r="AG34">
+        <v>0.89</v>
+      </c>
+      <c r="AH34">
+        <v>0.89</v>
+      </c>
+      <c r="AI34">
+        <v>0.89</v>
+      </c>
+      <c r="AJ34">
+        <v>0.89</v>
+      </c>
+      <c r="AK34">
+        <v>0.89</v>
+      </c>
+      <c r="AL34">
+        <v>0.89</v>
+      </c>
+      <c r="AM34">
+        <v>0.89</v>
+      </c>
+      <c r="AN34">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1906,8 +2673,62 @@
       <c r="P35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S35">
+        <v>15</v>
+      </c>
+      <c r="W35">
+        <v>0.94992187500000003</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
+      <c r="Z35">
+        <v>1</v>
+      </c>
+      <c r="AA35">
+        <v>1</v>
+      </c>
+      <c r="AB35">
+        <v>0.95</v>
+      </c>
+      <c r="AC35">
+        <v>0.95</v>
+      </c>
+      <c r="AD35">
+        <v>0.95</v>
+      </c>
+      <c r="AE35">
+        <v>0.95</v>
+      </c>
+      <c r="AF35">
+        <v>0.95</v>
+      </c>
+      <c r="AG35">
+        <v>0.95</v>
+      </c>
+      <c r="AH35">
+        <v>0.95</v>
+      </c>
+      <c r="AI35">
+        <v>0.95</v>
+      </c>
+      <c r="AJ35">
+        <v>0.95</v>
+      </c>
+      <c r="AK35">
+        <v>0.95</v>
+      </c>
+      <c r="AL35">
+        <v>0.95</v>
+      </c>
+      <c r="AM35">
+        <v>0.95</v>
+      </c>
+      <c r="AN35">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1956,8 +2777,65 @@
       <c r="P36">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S36">
+        <v>16</v>
+      </c>
+      <c r="T36">
+        <v>1.01325</v>
+      </c>
+      <c r="W36">
+        <v>1.01325</v>
+      </c>
+      <c r="Y36">
+        <v>1.01</v>
+      </c>
+      <c r="Z36">
+        <v>1.01</v>
+      </c>
+      <c r="AA36">
+        <v>1.01</v>
+      </c>
+      <c r="AB36">
+        <v>1.01</v>
+      </c>
+      <c r="AC36">
+        <v>1.01</v>
+      </c>
+      <c r="AD36">
+        <v>1.01</v>
+      </c>
+      <c r="AE36">
+        <v>1.01</v>
+      </c>
+      <c r="AF36">
+        <v>1.01</v>
+      </c>
+      <c r="AG36">
+        <v>1.01</v>
+      </c>
+      <c r="AH36">
+        <v>1.01</v>
+      </c>
+      <c r="AI36">
+        <v>1.01</v>
+      </c>
+      <c r="AJ36">
+        <v>1.01</v>
+      </c>
+      <c r="AK36">
+        <v>1.01</v>
+      </c>
+      <c r="AL36">
+        <v>1.01</v>
+      </c>
+      <c r="AM36">
+        <v>1.01</v>
+      </c>
+      <c r="AN36">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>ROUND(A1*A21, 2)</f>
         <v>24.23</v>
@@ -2023,7 +2901,7 @@
         <v>24.23</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" ref="A41:P55" si="1">ROUND(A2*A22, 2)</f>
         <v>48.47</v>
@@ -2089,7 +2967,7 @@
         <v>48.47</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>72.7</v>
@@ -2155,7 +3033,7 @@
         <v>72.7</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>96.94</v>
@@ -2221,7 +3099,7 @@
         <v>96.94</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>121.17</v>
@@ -2287,7 +3165,7 @@
         <v>121.17</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>145.41</v>
@@ -2353,7 +3231,7 @@
         <v>145.41</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>169.64</v>
@@ -2419,7 +3297,7 @@
         <v>169.64</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>193.88</v>
@@ -2485,7 +3363,7 @@
         <v>193.88</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>218.11</v>

</xml_diff>

<commit_message>
Calculations on MAP and TPS fail fix
</commit_message>
<xml_diff>
--- a/Docs/Injection table - precalculated.xlsx
+++ b/Docs/Injection table - precalculated.xlsx
@@ -359,13 +359,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N4" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21:AN36"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:AN16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>24.23</v>
       </c>
@@ -414,8 +414,72 @@
       <c r="P1">
         <v>24.23</v>
       </c>
+      <c r="Y1">
+        <f>Y21*100000</f>
+        <v>50000</v>
+      </c>
+      <c r="Z1">
+        <f t="shared" ref="Z1:AM1" si="0">Z21*100000</f>
+        <v>40000</v>
+      </c>
+      <c r="AA1">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="AB1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AC1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AD1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AE1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AF1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AG1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AH1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AI1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AJ1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AK1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AL1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AM1">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AN1">
+        <f>AN21*100000</f>
+        <v>6000</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>48.47</v>
       </c>
@@ -464,8 +528,72 @@
       <c r="P2">
         <v>48.47</v>
       </c>
+      <c r="Y2">
+        <f t="shared" ref="Y2:AM16" si="1">Y22*100000</f>
+        <v>50000</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="AA2">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AB2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AC2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AD2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AE2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AF2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AG2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AH2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AI2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AJ2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AK2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AL2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AM2">
+        <f t="shared" si="1"/>
+        <v>13000</v>
+      </c>
+      <c r="AN2">
+        <f t="shared" ref="AN2" si="2">AN22*100000</f>
+        <v>13000</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>72.7</v>
       </c>
@@ -514,8 +642,72 @@
       <c r="P3">
         <v>72.7</v>
       </c>
+      <c r="Y3">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AC3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AD3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AG3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AH3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AI3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AK3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" si="1"/>
+        <v>19000</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" ref="AN3" si="3">AN23*100000</f>
+        <v>19000</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>96.94</v>
       </c>
@@ -564,8 +756,72 @@
       <c r="P4">
         <v>96.94</v>
       </c>
+      <c r="Y4">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" si="1"/>
+        <v>35000</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AJ4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AK4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AL4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" ref="AN4" si="4">AN24*100000</f>
+        <v>25000</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>121.17</v>
       </c>
@@ -614,8 +870,72 @@
       <c r="P5">
         <v>121.17</v>
       </c>
+      <c r="Y5">
+        <f t="shared" si="1"/>
+        <v>55000.000000000007</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AJ5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" ref="AN5" si="5">AN25*100000</f>
+        <v>32000</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>145.41</v>
       </c>
@@ -664,8 +984,72 @@
       <c r="P6">
         <v>145.41</v>
       </c>
+      <c r="Y6">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="1"/>
+        <v>45000</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AJ6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AK6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AL6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" ref="AN6" si="6">AN26*100000</f>
+        <v>38000</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>169.64</v>
       </c>
@@ -714,8 +1098,72 @@
       <c r="P7">
         <v>169.64</v>
       </c>
+      <c r="Y7">
+        <f t="shared" si="1"/>
+        <v>65000</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AJ7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AK7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AL7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" ref="AN7" si="7">AN27*100000</f>
+        <v>44000</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>193.88</v>
       </c>
@@ -764,8 +1212,72 @@
       <c r="P8">
         <v>193.88</v>
       </c>
+      <c r="Y8">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="1"/>
+        <v>65000</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="1"/>
+        <v>65000</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AJ8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AK8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AL8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AM8">
+        <f t="shared" si="1"/>
+        <v>51000</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" ref="AN8" si="8">AN28*100000</f>
+        <v>51000</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>218.11</v>
       </c>
@@ -814,8 +1326,72 @@
       <c r="P9">
         <v>218.11</v>
       </c>
+      <c r="Y9">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AI9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AJ9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AK9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AL9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="1"/>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" ref="AN9" si="9">AN29*100000</f>
+        <v>56999.999999999993</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>242.34</v>
       </c>
@@ -864,8 +1440,72 @@
       <c r="P10">
         <v>242.34</v>
       </c>
+      <c r="Y10">
+        <f t="shared" si="1"/>
+        <v>90000</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AJ10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AK10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AL10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="1"/>
+        <v>63000</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" ref="AN10" si="10">AN30*100000</f>
+        <v>63000</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>266.58</v>
       </c>
@@ -914,8 +1554,72 @@
       <c r="P11">
         <v>266.58</v>
       </c>
+      <c r="Y11">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="1"/>
+        <v>90000</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="1"/>
+        <v>75000</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AI11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AJ11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AK11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AL11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AM11">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" ref="AN11" si="11">AN31*100000</f>
+        <v>70000</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>290.81</v>
       </c>
@@ -964,8 +1668,72 @@
       <c r="P12">
         <v>290.81</v>
       </c>
+      <c r="Y12">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="1"/>
+        <v>90000</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AJ12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AK12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AL12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" ref="AN12" si="12">AN32*100000</f>
+        <v>76000</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>315.05</v>
       </c>
@@ -1014,8 +1782,72 @@
       <c r="P13">
         <v>315.05</v>
       </c>
+      <c r="Y13">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="1"/>
+        <v>90000</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AI13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AJ13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AK13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AL13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AM13">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" ref="AN13" si="13">AN33*100000</f>
+        <v>82000</v>
+      </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>339.28</v>
       </c>
@@ -1064,8 +1896,72 @@
       <c r="P14">
         <v>339.28</v>
       </c>
+      <c r="Y14">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="1"/>
+        <v>97000</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AF14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AG14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AH14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AI14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AJ14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AK14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AL14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AM14">
+        <f t="shared" si="1"/>
+        <v>89000</v>
+      </c>
+      <c r="AN14">
+        <f t="shared" ref="AN14" si="14">AN34*100000</f>
+        <v>89000</v>
+      </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>363.52</v>
       </c>
@@ -1114,8 +2010,72 @@
       <c r="P15">
         <v>363.52</v>
       </c>
+      <c r="Y15">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AF15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AI15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AJ15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AK15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AL15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AM15">
+        <f t="shared" si="1"/>
+        <v>95000</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" ref="AN15" si="15">AN35*100000</f>
+        <v>95000</v>
+      </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>387.75</v>
       </c>
@@ -1163,6 +2123,70 @@
       </c>
       <c r="P16">
         <v>387.75</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AF16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AG16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AH16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AI16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AJ16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AK16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AL16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AM16">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+      <c r="AN16">
+        <f t="shared" ref="AN16" si="16">AN36*100000</f>
+        <v>101000</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
@@ -2841,1053 +3865,1053 @@
         <v>24.23</v>
       </c>
       <c r="B40">
-        <f t="shared" ref="B40:P40" si="0">ROUND(B1*B21, 2)</f>
+        <f t="shared" ref="B40:P40" si="17">ROUND(B1*B21, 2)</f>
         <v>24.23</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="D40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="H40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="I40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="J40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="K40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="L40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="M40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="N40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="O40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
       <c r="P40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="17"/>
         <v>24.23</v>
       </c>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" ref="A41:P55" si="1">ROUND(A2*A22, 2)</f>
+        <f t="shared" ref="A41:P55" si="18">ROUND(A2*A22, 2)</f>
         <v>48.47</v>
       </c>
       <c r="B41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="G41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="H41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="I41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="J41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="K41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="L41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="M41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="N41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="O41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
       <c r="P41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>48.47</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="B42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="E42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="F42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="H42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="I42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="J42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="K42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="L42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="M42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="N42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="O42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
       <c r="P42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>72.7</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="B43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="E43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="F43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="G43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="H43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="I43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="J43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="K43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="L43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="M43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="N43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="O43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
       <c r="P43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>96.94</v>
       </c>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="B44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="D44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="E44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="H44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="I44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="J44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="K44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="L44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="M44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="N44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="O44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
       <c r="P44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>121.17</v>
       </c>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="B45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="E45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="F45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="G45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="H45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="I45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="J45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="K45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="L45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="M45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="N45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="O45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
       <c r="P45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>145.41</v>
       </c>
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="B46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="D46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="E46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="F46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="H46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="I46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="J46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="K46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="L46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="M46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="N46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="O46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
       <c r="P46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>169.64</v>
       </c>
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="B47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="D47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="E47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="F47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="G47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="H47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="I47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="J47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="K47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="L47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="M47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="N47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="O47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
       <c r="P47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>193.88</v>
       </c>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="B48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="D48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="E48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="G48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="H48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="I48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="J48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="K48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="L48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="M48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="N48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="O48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
       <c r="P48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>218.11</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="B49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="D49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="E49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="F49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="G49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="H49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="I49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="J49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="K49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="L49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="M49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="N49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="O49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
       <c r="P49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>242.34</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="B50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="D50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="E50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="F50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="G50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="H50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="I50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="J50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="K50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="L50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="M50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="N50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="O50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
       <c r="P50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>266.58</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="B51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="D51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="E51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="F51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="G51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="H51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="I51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="J51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="K51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="L51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="M51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="N51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="O51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
       <c r="P51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>290.81</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="B52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="C52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="D52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="E52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="F52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="G52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="H52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="I52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="J52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="K52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="L52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="M52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="N52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="O52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
       <c r="P52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>315.05</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="B53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="C53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="D53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="E53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="F53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="G53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="H53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="I53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="J53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="K53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="L53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="M53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="N53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="O53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
       <c r="P53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>339.28</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="B54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="C54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="D54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="E54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="F54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="G54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="H54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="I54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="J54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="K54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="L54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="M54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="N54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="O54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
       <c r="P54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>363.52</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="B55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="C55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="D55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="E55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="F55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="G55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="H55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="I55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="J55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="K55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="L55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="M55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="N55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="O55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
       <c r="P55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>387.75</v>
       </c>
     </row>

</xml_diff>